<commit_message>
Add courses.xlsx using repos version of courses.xlsx
</commit_message>
<xml_diff>
--- a/navisewebsite/courses.xlsx
+++ b/navisewebsite/courses.xlsx
@@ -8,18 +8,18 @@
   <sheets>
     <sheet name="ArtSheet" r:id="rId3" sheetId="1"/>
     <sheet name="FallCourses" r:id="rId4" sheetId="2"/>
-    <sheet name="SpringCourses" r:id="rId5" sheetId="3"/>
-    <sheet name="FallSheet" r:id="rId6" sheetId="4"/>
-    <sheet name="SpringSheet" r:id="rId7" sheetId="5"/>
-    <sheet name="ChemSheet" r:id="rId8" sheetId="6"/>
-    <sheet name="MathSheet" r:id="rId9" sheetId="7"/>
-    <sheet name="BioSheet" r:id="rId10" sheetId="8"/>
+    <sheet name="FallSheet" r:id="rId5" sheetId="3"/>
+    <sheet name="SpringSheet" r:id="rId6" sheetId="4"/>
+    <sheet name="ChemSheet" r:id="rId7" sheetId="5"/>
+    <sheet name="MathSheet" r:id="rId8" sheetId="6"/>
+    <sheet name="BioSheet" r:id="rId9" sheetId="7"/>
+    <sheet name="SpringCourses" r:id="rId10" sheetId="8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="87">
   <si>
     <t>CourseID</t>
   </si>
@@ -144,142 +144,142 @@
     <t>CS102</t>
   </si>
   <si>
+    <t>C501</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>HIST101</t>
+  </si>
+  <si>
+    <t>Prof H</t>
+  </si>
+  <si>
+    <t>Building1</t>
+  </si>
+  <si>
+    <t>501</t>
+  </si>
+  <si>
+    <t>C502</t>
+  </si>
+  <si>
+    <t>History2</t>
+  </si>
+  <si>
+    <t>HIST102</t>
+  </si>
+  <si>
+    <t>Prof I</t>
+  </si>
+  <si>
+    <t>Building2</t>
+  </si>
+  <si>
+    <t>502</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>C401</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>CHEM101</t>
+  </si>
+  <si>
+    <t>Prof Chem</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>LabRequired, SafetyTraining</t>
+  </si>
+  <si>
+    <t>C201</t>
+  </si>
+  <si>
+    <t>Math1</t>
+  </si>
+  <si>
+    <t>MATH101</t>
+  </si>
+  <si>
+    <t>Prof X</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>C202</t>
+  </si>
+  <si>
+    <t>Math2</t>
+  </si>
+  <si>
+    <t>MATH102</t>
+  </si>
+  <si>
+    <t>Prof Y</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>C601</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>BIO101</t>
+  </si>
+  <si>
+    <t>Prof Bio</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>BioBuilding</t>
+  </si>
+  <si>
+    <t>601</t>
+  </si>
+  <si>
+    <t>C101</t>
+  </si>
+  <si>
+    <t>Intro to CS</t>
+  </si>
+  <si>
+    <t>CS101</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
     <t>C102</t>
   </si>
   <si>
     <t>Data Structures</t>
   </si>
   <si>
-    <t>10:00</t>
-  </si>
-  <si>
     <t>102</t>
-  </si>
-  <si>
-    <t>C101</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>C501</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>HIST101</t>
-  </si>
-  <si>
-    <t>Prof H</t>
-  </si>
-  <si>
-    <t>Building1</t>
-  </si>
-  <si>
-    <t>501</t>
-  </si>
-  <si>
-    <t>C502</t>
-  </si>
-  <si>
-    <t>History2</t>
-  </si>
-  <si>
-    <t>HIST102</t>
-  </si>
-  <si>
-    <t>Prof I</t>
-  </si>
-  <si>
-    <t>Building2</t>
-  </si>
-  <si>
-    <t>502</t>
-  </si>
-  <si>
-    <t>C401</t>
-  </si>
-  <si>
-    <t>Chemistry</t>
-  </si>
-  <si>
-    <t>CHEM101</t>
-  </si>
-  <si>
-    <t>Prof Chem</t>
-  </si>
-  <si>
-    <t>14:00</t>
-  </si>
-  <si>
-    <t>Lab</t>
-  </si>
-  <si>
-    <t>401</t>
-  </si>
-  <si>
-    <t>LabRequired, SafetyTraining</t>
-  </si>
-  <si>
-    <t>C201</t>
-  </si>
-  <si>
-    <t>Math1</t>
-  </si>
-  <si>
-    <t>MATH101</t>
-  </si>
-  <si>
-    <t>Prof X</t>
-  </si>
-  <si>
-    <t>Science</t>
-  </si>
-  <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>C202</t>
-  </si>
-  <si>
-    <t>Math2</t>
-  </si>
-  <si>
-    <t>MATH102</t>
-  </si>
-  <si>
-    <t>Prof Y</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>C601</t>
-  </si>
-  <si>
-    <t>Biology</t>
-  </si>
-  <si>
-    <t>BIO101</t>
-  </si>
-  <si>
-    <t>Prof Bio</t>
-  </si>
-  <si>
-    <t>BioBuilding</t>
-  </si>
-  <si>
-    <t>601</t>
-  </si>
-  <si>
-    <t>Intro to CS</t>
-  </si>
-  <si>
-    <t>CS101</t>
-  </si>
-  <si>
-    <t>101</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,13 +427,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>3.0</v>
@@ -451,7 +451,7 @@
         <v>37</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J2" t="s" s="0">
         <v>21</v>
@@ -463,6 +463,88 @@
         <v>22</v>
       </c>
       <c r="M2" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s" s="0">
         <v>23</v>
       </c>
     </row>
@@ -473,7 +555,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -528,37 +610,119 @@
         <v>42</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="H2" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="I2" t="s" s="0">
+      <c r="D3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="K2" t="s" s="0">
+      <c r="F3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="L2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s" s="0">
+      <c r="I3" t="s" s="0">
         <v>46</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -568,7 +732,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -632,10 +796,10 @@
         <v>50</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>51</v>
@@ -644,7 +808,7 @@
         <v>52</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>22</v>
@@ -653,7 +817,89 @@
         <v>22</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>23</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -663,7 +909,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -712,43 +958,125 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>3.0</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>28</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="F3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="K2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s" s="0">
-        <v>46</v>
+      <c r="H3" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +1086,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -807,43 +1135,248 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>3.0</v>
       </c>
       <c r="E2" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="L3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G5" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="C6" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="D6" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="F6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="K2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s" s="0">
-        <v>46</v>
+      <c r="I6" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="K7" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -853,7 +1386,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -902,34 +1435,34 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>17</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="K2" t="s" s="0">
         <v>22</v>
@@ -952,34 +1485,75 @@
         <v>75</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>76</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="J3" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="L3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="M3" t="s" s="0">
-        <v>46</v>
+      <c r="H4" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1038,43 +1612,43 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D2" t="n" s="0">
         <v>4.0</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="L2" t="s" s="0">
         <v>22</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>